<commit_message>
finished bar chart with dropdowns
</commit_message>
<xml_diff>
--- a/rawdata/codebook.xlsx
+++ b/rawdata/codebook.xlsx
@@ -8372,7 +8372,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{AF02DEB3-6639-4AD6-BB0C-3B72EFE01D8B}" name="rabest265@gmail.com" id="-1876340319" dateTime="2019-06-19T00:27:41"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>